<commit_message>
added payroll for machine csv
</commit_message>
<xml_diff>
--- a/processed_files/INVOICE - 2023-08-01 - 2023-08-15.xlsx
+++ b/processed_files/INVOICE - 2023-08-01 - 2023-08-15.xlsx
@@ -830,7 +830,7 @@
         </is>
       </c>
       <c r="C8" s="26" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D8" s="26" t="n">
         <v>2023</v>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="C40" s="61" t="inlineStr">
         <is>
-          <t>08.17.23</t>
+          <t>08.21.23</t>
         </is>
       </c>
       <c r="D40" s="58" t="n"/>

</xml_diff>